<commit_message>
exculde Bắc Kinh với Thượng Hải, Osaka
</commit_message>
<xml_diff>
--- a/nuoc_ngoai/forecast_results.xlsx
+++ b/nuoc_ngoai/forecast_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BS8"/>
+  <dimension ref="A1:BD8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,150 +641,75 @@
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>Bắc Kinh (Trung Quốc) - Linear Regression</t>
+          <t>Thâm Quyến (Trung Quốc) - Linear Regression</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>Bắc Kinh (Trung Quốc) - Prophet</t>
+          <t>Thâm Quyến (Trung Quốc) - Prophet</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>Bắc Kinh (Trung Quốc) - 10% Growth</t>
+          <t>Thâm Quyến (Trung Quốc) - 10% Growth</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>Bắc Kinh (Trung Quốc) - GDP Growth</t>
+          <t>Thâm Quyến (Trung Quốc) - GDP Growth</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>Bắc Kinh (Trung Quốc) - Exponential Smoothing</t>
+          <t>Thâm Quyến (Trung Quốc) - Exponential Smoothing</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>Thượng Hải (Trung Quốc) - Linear Regression</t>
+          <t>Osaka (Nhật Bản) - Linear Regression</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>Thượng Hải (Trung Quốc) - Prophet</t>
+          <t>Osaka (Nhật Bản) - Prophet</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>Thượng Hải (Trung Quốc) - 10% Growth</t>
+          <t>Osaka (Nhật Bản) - 10% Growth</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>Thượng Hải (Trung Quốc) - GDP Growth</t>
+          <t>Osaka (Nhật Bản) - GDP Growth</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>Thượng Hải (Trung Quốc) - Exponential Smoothing</t>
+          <t>Osaka (Nhật Bản) - Exponential Smoothing</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>Thâm Quyến (Trung Quốc) - Linear Regression</t>
+          <t>TP. Hồ Chí Minh (Việt Nam) - Linear Regression</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>Thâm Quyến (Trung Quốc) - Prophet</t>
+          <t>TP. Hồ Chí Minh (Việt Nam) - Prophet</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>Thâm Quyến (Trung Quốc) - 10% Growth</t>
+          <t>TP. Hồ Chí Minh (Việt Nam) - 10% Growth</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>Thâm Quyến (Trung Quốc) - GDP Growth</t>
+          <t>TP. Hồ Chí Minh (Việt Nam) - GDP Growth</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
-        <is>
-          <t>Thâm Quyến (Trung Quốc) - Exponential Smoothing</t>
-        </is>
-      </c>
-      <c r="BE1" s="1" t="inlineStr">
-        <is>
-          <t>Tokyo (Nhật Bản) - Linear Regression</t>
-        </is>
-      </c>
-      <c r="BF1" s="1" t="inlineStr">
-        <is>
-          <t>Tokyo (Nhật Bản) - Prophet</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
-          <t>Tokyo (Nhật Bản) - 10% Growth</t>
-        </is>
-      </c>
-      <c r="BH1" s="1" t="inlineStr">
-        <is>
-          <t>Tokyo (Nhật Bản) - GDP Growth</t>
-        </is>
-      </c>
-      <c r="BI1" s="1" t="inlineStr">
-        <is>
-          <t>Tokyo (Nhật Bản) - Exponential Smoothing</t>
-        </is>
-      </c>
-      <c r="BJ1" s="1" t="inlineStr">
-        <is>
-          <t>Osaka (Nhật Bản) - Linear Regression</t>
-        </is>
-      </c>
-      <c r="BK1" s="1" t="inlineStr">
-        <is>
-          <t>Osaka (Nhật Bản) - Prophet</t>
-        </is>
-      </c>
-      <c r="BL1" s="1" t="inlineStr">
-        <is>
-          <t>Osaka (Nhật Bản) - 10% Growth</t>
-        </is>
-      </c>
-      <c r="BM1" s="1" t="inlineStr">
-        <is>
-          <t>Osaka (Nhật Bản) - GDP Growth</t>
-        </is>
-      </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>Osaka (Nhật Bản) - Exponential Smoothing</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
-        <is>
-          <t>TP. Hồ Chí Minh (Việt Nam) - Linear Regression</t>
-        </is>
-      </c>
-      <c r="BP1" s="1" t="inlineStr">
-        <is>
-          <t>TP. Hồ Chí Minh (Việt Nam) - Prophet</t>
-        </is>
-      </c>
-      <c r="BQ1" s="1" t="inlineStr">
-        <is>
-          <t>TP. Hồ Chí Minh (Việt Nam) - 10% Growth</t>
-        </is>
-      </c>
-      <c r="BR1" s="1" t="inlineStr">
-        <is>
-          <t>TP. Hồ Chí Minh (Việt Nam) - GDP Growth</t>
-        </is>
-      </c>
-      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>TP. Hồ Chí Minh (Việt Nam) - Exponential Smoothing</t>
         </is>
@@ -915,93 +840,48 @@
         <v>108.1999999586922</v>
       </c>
       <c r="AP2" t="n">
-        <v>729.9100000000035</v>
+        <v>535.0400000000081</v>
       </c>
       <c r="AQ2" t="n">
-        <v>729.9253492646075</v>
+        <v>535.0280096835123</v>
       </c>
       <c r="AR2" t="n">
-        <v>739.2</v>
+        <v>550</v>
       </c>
       <c r="AS2" t="n">
-        <v>712.3927960721803</v>
+        <v>530.0541637441818</v>
       </c>
       <c r="AT2" t="n">
-        <v>729.9099912405995</v>
+        <v>535.0401736812117</v>
       </c>
       <c r="AU2" t="n">
-        <v>631</v>
+        <v>261.8399999999965</v>
       </c>
       <c r="AV2" t="n">
-        <v>631.0243940639606</v>
+        <v>276.1685757024036</v>
       </c>
       <c r="AW2" t="n">
-        <v>671</v>
+        <v>319</v>
       </c>
       <c r="AX2" t="n">
-        <v>646.6660797679018</v>
+        <v>278.2688073256447</v>
       </c>
       <c r="AY2" t="n">
-        <v>630.9999391355766</v>
+        <v>261.8398708902199</v>
       </c>
       <c r="AZ2" t="n">
-        <v>535.0400000000081</v>
+        <v>98.49620779999896</v>
       </c>
       <c r="BA2" t="n">
-        <v>535.0280096835123</v>
+        <v>98.50737416353002</v>
       </c>
       <c r="BB2" t="n">
-        <v>550</v>
+        <v>105.79415</v>
       </c>
       <c r="BC2" t="n">
-        <v>530.0541637441818</v>
+        <v>103.87062</v>
       </c>
       <c r="BD2" t="n">
-        <v>535.0401736812117</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>843.4799999999959</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>839.5532982848666</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>979.0000000000001</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>853.9973742062889</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>843.4799989637395</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>261.8399999999965</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>276.1685757024036</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>319</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>278.2688073256447</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>261.8398708902199</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>98.49620779999896</v>
-      </c>
-      <c r="BP2" t="n">
-        <v>98.50737416353002</v>
-      </c>
-      <c r="BQ2" t="n">
-        <v>105.79415</v>
-      </c>
-      <c r="BR2" t="n">
-        <v>103.87062</v>
-      </c>
-      <c r="BS2" t="n">
         <v>98.49620487933093</v>
       </c>
     </row>
@@ -1130,93 +1010,48 @@
         <v>111.999999952278</v>
       </c>
       <c r="AP3" t="n">
-        <v>780.7800000000134</v>
+        <v>568.3600000000006</v>
       </c>
       <c r="AQ3" t="n">
-        <v>780.7535466241571</v>
+        <v>568.3108362666585</v>
       </c>
       <c r="AR3" t="n">
-        <v>813.1200000000001</v>
+        <v>605.0000000000001</v>
       </c>
       <c r="AS3" t="n">
-        <v>755.213535558838</v>
+        <v>561.9148330050879</v>
       </c>
       <c r="AT3" t="n">
-        <v>780.7799861760591</v>
+        <v>568.3602155939217</v>
       </c>
       <c r="AU3" t="n">
-        <v>650</v>
+        <v>239.2599999999948</v>
       </c>
       <c r="AV3" t="n">
-        <v>650.0148694081661</v>
+        <v>263.1552828599827</v>
       </c>
       <c r="AW3" t="n">
-        <v>738.1000000000001</v>
+        <v>350.9</v>
       </c>
       <c r="AX3" t="n">
-        <v>685.5360962662071</v>
+        <v>267.0121694152992</v>
       </c>
       <c r="AY3" t="n">
-        <v>649.9999198098872</v>
+        <v>239.2598218683942</v>
       </c>
       <c r="AZ3" t="n">
-        <v>568.3600000000006</v>
+        <v>103.0690156000001</v>
       </c>
       <c r="BA3" t="n">
-        <v>568.3108362666585</v>
+        <v>103.0826699901492</v>
       </c>
       <c r="BB3" t="n">
-        <v>605.0000000000001</v>
+        <v>116.373565</v>
       </c>
       <c r="BC3" t="n">
-        <v>561.9148330050879</v>
+        <v>112.1802696</v>
       </c>
       <c r="BD3" t="n">
-        <v>568.3602155939217</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>799.2199999999866</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>793.1913938654964</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>1076.9</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>819.4511406193666</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>799.219998473307</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>239.2599999999948</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>263.1552828599827</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>350.9</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>267.0121694152992</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>239.2598218683942</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>103.0690156000001</v>
-      </c>
-      <c r="BP3" t="n">
-        <v>103.0826699901492</v>
-      </c>
-      <c r="BQ3" t="n">
-        <v>116.373565</v>
-      </c>
-      <c r="BR3" t="n">
-        <v>112.1802696</v>
-      </c>
-      <c r="BS3" t="n">
         <v>103.0690114036274</v>
       </c>
     </row>
@@ -1345,93 +1180,48 @@
         <v>115.7999999458639</v>
       </c>
       <c r="AP4" t="n">
-        <v>831.6500000000087</v>
+        <v>601.6800000000076</v>
       </c>
       <c r="AQ4" t="n">
-        <v>831.5817439837065</v>
+        <v>601.5936628498047</v>
       </c>
       <c r="AR4" t="n">
-        <v>894.4320000000002</v>
+        <v>665.5000000000002</v>
       </c>
       <c r="AS4" t="n">
-        <v>800.6081580778535</v>
+        <v>595.6905938079268</v>
       </c>
       <c r="AT4" t="n">
-        <v>831.6499811115185</v>
+        <v>601.6802575066317</v>
       </c>
       <c r="AU4" t="n">
-        <v>669</v>
+        <v>216.6800000000003</v>
       </c>
       <c r="AV4" t="n">
-        <v>669.0053447523717</v>
+        <v>250.1419900175619</v>
       </c>
       <c r="AW4" t="n">
-        <v>811.9100000000002</v>
+        <v>385.9900000000001</v>
       </c>
       <c r="AX4" t="n">
-        <v>726.7425244456707</v>
+        <v>256.21088939527</v>
       </c>
       <c r="AY4" t="n">
-        <v>668.9999004841978</v>
+        <v>216.6797728465687</v>
       </c>
       <c r="AZ4" t="n">
-        <v>601.6800000000076</v>
+        <v>107.6418233999993</v>
       </c>
       <c r="BA4" t="n">
-        <v>601.5936628498047</v>
+        <v>107.6579658167683</v>
       </c>
       <c r="BB4" t="n">
-        <v>665.5000000000002</v>
+        <v>128.0109215000001</v>
       </c>
       <c r="BC4" t="n">
-        <v>595.6905938079268</v>
+        <v>121.154691168</v>
       </c>
       <c r="BD4" t="n">
-        <v>601.6802575066317</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>754.9599999999919</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>746.8294894461261</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>1184.59</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>786.3023846958287</v>
-      </c>
-      <c r="BI4" t="n">
-        <v>754.9599979828745</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>216.6800000000003</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>250.1419900175619</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>385.9900000000001</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>256.21088939527</v>
-      </c>
-      <c r="BN4" t="n">
-        <v>216.6797728465687</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>107.6418233999993</v>
-      </c>
-      <c r="BP4" t="n">
-        <v>107.6579658167683</v>
-      </c>
-      <c r="BQ4" t="n">
-        <v>128.0109215000001</v>
-      </c>
-      <c r="BR4" t="n">
-        <v>121.154691168</v>
-      </c>
-      <c r="BS4" t="n">
         <v>107.6418179279238</v>
       </c>
     </row>
@@ -1560,93 +1350,48 @@
         <v>119.5999999394497</v>
       </c>
       <c r="AP5" t="n">
-        <v>882.5200000000041</v>
+        <v>635</v>
       </c>
       <c r="AQ5" t="n">
-        <v>882.4099413432562</v>
+        <v>634.8764894329508</v>
       </c>
       <c r="AR5" t="n">
-        <v>983.8752000000003</v>
+        <v>732.0500000000002</v>
       </c>
       <c r="AS5" t="n">
-        <v>848.7313754334526</v>
+        <v>631.4965591022714</v>
       </c>
       <c r="AT5" t="n">
-        <v>882.5199760469779</v>
+        <v>635.0002994193418</v>
       </c>
       <c r="AU5" t="n">
-        <v>688</v>
+        <v>194.0999999999985</v>
       </c>
       <c r="AV5" t="n">
-        <v>687.9958200965772</v>
+        <v>237.128697175141</v>
       </c>
       <c r="AW5" t="n">
-        <v>893.1010000000002</v>
+        <v>424.5890000000001</v>
       </c>
       <c r="AX5" t="n">
-        <v>770.425802104771</v>
+        <v>245.8465469512568</v>
       </c>
       <c r="AY5" t="n">
-        <v>687.9998811585084</v>
+        <v>194.0997238247431</v>
       </c>
       <c r="AZ5" t="n">
-        <v>635</v>
+        <v>112.2146312000004</v>
       </c>
       <c r="BA5" t="n">
-        <v>634.8764894329508</v>
+        <v>112.2332616433875</v>
       </c>
       <c r="BB5" t="n">
-        <v>732.0500000000002</v>
+        <v>140.81201365</v>
       </c>
       <c r="BC5" t="n">
-        <v>631.4965591022714</v>
+        <v>130.84706646144</v>
       </c>
       <c r="BD5" t="n">
-        <v>635.0002994193418</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>710.6999999999971</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>700.4675850267558</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>1303.049</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>754.4945751262708</v>
-      </c>
-      <c r="BI5" t="n">
-        <v>710.699997492442</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>194.0999999999985</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>237.128697175141</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>424.5890000000001</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>245.8465469512568</v>
-      </c>
-      <c r="BN5" t="n">
-        <v>194.0997238247431</v>
-      </c>
-      <c r="BO5" t="n">
-        <v>112.2146312000004</v>
-      </c>
-      <c r="BP5" t="n">
-        <v>112.2332616433875</v>
-      </c>
-      <c r="BQ5" t="n">
-        <v>140.81201365</v>
-      </c>
-      <c r="BR5" t="n">
-        <v>130.84706646144</v>
-      </c>
-      <c r="BS5" t="n">
         <v>112.2146244522202</v>
       </c>
     </row>
@@ -1775,93 +1520,48 @@
         <v>123.3999999330355</v>
       </c>
       <c r="AP6" t="n">
-        <v>933.390000000014</v>
+        <v>668.320000000007</v>
       </c>
       <c r="AQ6" t="n">
-        <v>933.3773940380372</v>
+        <v>668.2505018423523</v>
       </c>
       <c r="AR6" t="n">
-        <v>1082.26272</v>
+        <v>805.2550000000002</v>
       </c>
       <c r="AS6" t="n">
-        <v>899.7471988976559</v>
+        <v>669.4547610845655</v>
       </c>
       <c r="AT6" t="n">
-        <v>933.3899709824374</v>
+        <v>668.3203413320518</v>
       </c>
       <c r="AU6" t="n">
-        <v>707</v>
+        <v>171.5199999999968</v>
       </c>
       <c r="AV6" t="n">
-        <v>707.0383241403559</v>
+        <v>224.0797514756176</v>
       </c>
       <c r="AW6" t="n">
-        <v>982.4111000000004</v>
+        <v>467.0479000000001</v>
       </c>
       <c r="AX6" t="n">
-        <v>816.7348085231699</v>
+        <v>235.9014669146701</v>
       </c>
       <c r="AY6" t="n">
-        <v>706.999861832819</v>
+        <v>171.5196748029175</v>
       </c>
       <c r="AZ6" t="n">
-        <v>668.320000000007</v>
+        <v>116.7874389999997</v>
       </c>
       <c r="BA6" t="n">
-        <v>668.2505018423523</v>
+        <v>116.8210925270659</v>
       </c>
       <c r="BB6" t="n">
-        <v>805.2550000000002</v>
+        <v>154.8932150150001</v>
       </c>
       <c r="BC6" t="n">
-        <v>669.4547610845655</v>
+        <v>141.3148317783553</v>
       </c>
       <c r="BD6" t="n">
-        <v>668.3203413320518</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>666.4399999999878</v>
-      </c>
-      <c r="BF6" t="n">
-        <v>653.9786616911682</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>1433.353900000001</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>723.9734674277806</v>
-      </c>
-      <c r="BI6" t="n">
-        <v>666.4399970020095</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>171.5199999999968</v>
-      </c>
-      <c r="BK6" t="n">
-        <v>224.0797514756176</v>
-      </c>
-      <c r="BL6" t="n">
-        <v>467.0479000000001</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>235.9014669146701</v>
-      </c>
-      <c r="BN6" t="n">
-        <v>171.5196748029175</v>
-      </c>
-      <c r="BO6" t="n">
-        <v>116.7874389999997</v>
-      </c>
-      <c r="BP6" t="n">
-        <v>116.8210925270659</v>
-      </c>
-      <c r="BQ6" t="n">
-        <v>154.8932150150001</v>
-      </c>
-      <c r="BR6" t="n">
-        <v>141.3148317783553</v>
-      </c>
-      <c r="BS6" t="n">
         <v>116.7874309765166</v>
       </c>
     </row>
@@ -1990,93 +1690,48 @@
         <v>127.1999999266214</v>
       </c>
       <c r="AP7" t="n">
-        <v>984.2600000000093</v>
+        <v>701.6399999999994</v>
       </c>
       <c r="AQ7" t="n">
-        <v>984.2055913975867</v>
+        <v>701.5333284254984</v>
       </c>
       <c r="AR7" t="n">
-        <v>1190.488992000001</v>
+        <v>885.7805000000004</v>
       </c>
       <c r="AS7" t="n">
-        <v>953.829498185734</v>
+        <v>709.6945671024807</v>
       </c>
       <c r="AT7" t="n">
-        <v>984.2599659178968</v>
+        <v>701.6403832447618</v>
       </c>
       <c r="AU7" t="n">
-        <v>726</v>
+        <v>148.9399999999951</v>
       </c>
       <c r="AV7" t="n">
-        <v>726.0287994845615</v>
+        <v>211.0664586331968</v>
       </c>
       <c r="AW7" t="n">
-        <v>1080.65221</v>
+        <v>513.7526900000003</v>
       </c>
       <c r="AX7" t="n">
-        <v>865.8273718650264</v>
+        <v>226.3586891197079</v>
       </c>
       <c r="AY7" t="n">
-        <v>725.9998425071295</v>
+        <v>148.9396257810919</v>
       </c>
       <c r="AZ7" t="n">
-        <v>701.6399999999994</v>
+        <v>121.360246799999</v>
       </c>
       <c r="BA7" t="n">
-        <v>701.5333284254984</v>
+        <v>121.3963883536851</v>
       </c>
       <c r="BB7" t="n">
-        <v>885.7805000000004</v>
+        <v>170.3825365165001</v>
       </c>
       <c r="BC7" t="n">
-        <v>709.6945671024807</v>
+        <v>152.6200183206237</v>
       </c>
       <c r="BD7" t="n">
-        <v>701.6403832447618</v>
-      </c>
-      <c r="BE7" t="n">
-        <v>622.179999999993</v>
-      </c>
-      <c r="BF7" t="n">
-        <v>607.6167572717978</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>1576.689290000001</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>694.6870114363448</v>
-      </c>
-      <c r="BI7" t="n">
-        <v>622.1799965115771</v>
-      </c>
-      <c r="BJ7" t="n">
-        <v>148.9399999999951</v>
-      </c>
-      <c r="BK7" t="n">
-        <v>211.0664586331968</v>
-      </c>
-      <c r="BL7" t="n">
-        <v>513.7526900000003</v>
-      </c>
-      <c r="BM7" t="n">
-        <v>226.3586891197079</v>
-      </c>
-      <c r="BN7" t="n">
-        <v>148.9396257810919</v>
-      </c>
-      <c r="BO7" t="n">
-        <v>121.360246799999</v>
-      </c>
-      <c r="BP7" t="n">
-        <v>121.3963883536851</v>
-      </c>
-      <c r="BQ7" t="n">
-        <v>170.3825365165001</v>
-      </c>
-      <c r="BR7" t="n">
-        <v>152.6200183206237</v>
-      </c>
-      <c r="BS7" t="n">
         <v>121.360237500813</v>
       </c>
     </row>
@@ -2205,93 +1860,48 @@
         <v>130.9999999202072</v>
       </c>
       <c r="AP8" t="n">
-        <v>1035.130000000005</v>
+        <v>734.9600000000064</v>
       </c>
       <c r="AQ8" t="n">
-        <v>1035.033788757136</v>
+        <v>734.8161550086447</v>
       </c>
       <c r="AR8" t="n">
-        <v>1309.537891200001</v>
+        <v>974.3585500000006</v>
       </c>
       <c r="AS8" t="n">
-        <v>1011.162594030744</v>
+        <v>752.353120558589</v>
       </c>
       <c r="AT8" t="n">
-        <v>1035.129960853356</v>
+        <v>734.9604251574718</v>
       </c>
       <c r="AU8" t="n">
-        <v>745</v>
+        <v>126.3600000000006</v>
       </c>
       <c r="AV8" t="n">
-        <v>745.0192748287673</v>
+        <v>198.0531657907759</v>
       </c>
       <c r="AW8" t="n">
-        <v>1188.717431000001</v>
+        <v>565.1279590000004</v>
       </c>
       <c r="AX8" t="n">
-        <v>917.8708070814787</v>
+        <v>217.2019394797845</v>
       </c>
       <c r="AY8" t="n">
-        <v>744.9998231814402</v>
+        <v>126.3595767592663</v>
       </c>
       <c r="AZ8" t="n">
-        <v>734.9600000000064</v>
+        <v>125.9330546000001</v>
       </c>
       <c r="BA8" t="n">
-        <v>734.8161550086447</v>
+        <v>125.9716841803042</v>
       </c>
       <c r="BB8" t="n">
-        <v>974.3585500000006</v>
+        <v>187.4207901681501</v>
       </c>
       <c r="BC8" t="n">
-        <v>752.353120558589</v>
+        <v>164.8296197862736</v>
       </c>
       <c r="BD8" t="n">
-        <v>734.9604251574718</v>
-      </c>
-      <c r="BE8" t="n">
-        <v>577.9199999999837</v>
-      </c>
-      <c r="BF8" t="n">
-        <v>561.2548528524277</v>
-      </c>
-      <c r="BG8" t="n">
-        <v>1734.358219000001</v>
-      </c>
-      <c r="BH8" t="n">
-        <v>666.5852625414076</v>
-      </c>
-      <c r="BI8" t="n">
-        <v>577.9199960211446</v>
-      </c>
-      <c r="BJ8" t="n">
-        <v>126.3600000000006</v>
-      </c>
-      <c r="BK8" t="n">
-        <v>198.0531657907759</v>
-      </c>
-      <c r="BL8" t="n">
-        <v>565.1279590000004</v>
-      </c>
-      <c r="BM8" t="n">
-        <v>217.2019394797845</v>
-      </c>
-      <c r="BN8" t="n">
-        <v>126.3595767592663</v>
-      </c>
-      <c r="BO8" t="n">
-        <v>125.9330546000001</v>
-      </c>
-      <c r="BP8" t="n">
-        <v>125.9716841803042</v>
-      </c>
-      <c r="BQ8" t="n">
-        <v>187.4207901681501</v>
-      </c>
-      <c r="BR8" t="n">
-        <v>164.8296197862736</v>
-      </c>
-      <c r="BS8" t="n">
         <v>125.9330440251095</v>
       </c>
     </row>

</xml_diff>